<commit_message>
Add robustness for networks trained with noise
Three very simple robustness metrics were used:
confidences: expected confidence for correctly classified samples
misleads: expected misleading probability for misclassified samples
prob_groundtruths: probability for ground truth category when
misclassified
noise_count: average number of test samples (total 10,000) that are
misclassified to the extra noise category
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Accuracy" sheetId="1" r:id="rId1"/>
+    <sheet name="Robustness" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Rate of noise</t>
   </si>
@@ -83,6 +84,33 @@
   </si>
   <si>
     <t>10000</t>
+  </si>
+  <si>
+    <t>Average confidence for correctly classified samples</t>
+  </si>
+  <si>
+    <t>Average misleading probability for misclassified samples</t>
+  </si>
+  <si>
+    <t>Average probability of ground truth category for misclassified samples</t>
+  </si>
+  <si>
+    <t>Average number of noise for misclassified samples (not normalized)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>83.12%, 83.67%</t>
+  </si>
+  <si>
+    <t>59.56%, 59.49%</t>
+  </si>
+  <si>
+    <t>16.61%, 16.61%</t>
+  </si>
+  <si>
+    <t>0.06, 0.04</t>
   </si>
 </sst>
 </file>
@@ -437,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,13 +489,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -675,4 +703,149 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.83220000000000005</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.59389999999999998</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.16489999999999999</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.83509999999999995</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.1661</v>
+      </c>
+      <c r="E3">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.84140000000000004</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.59609999999999996</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.16589999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.84189999999999998</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.59509999999999996</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.1663</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.84209999999999996</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.5927</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.08</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Retrain the network with selected training samples
Percentage = 0.5.
For correctly classified training samples, we divide them to
high-confidence and low-confidence.
For misclassified training samples, we divide them to high-mislead and
low-mislead.
Four combinations of training samples were used:
low-confidence + low-mislead;
low-confidence + high-mislead;
high-confidence + low-mislead;
high-confidence + high-mislead.
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Test Accuracy" sheetId="1" r:id="rId1"/>
     <sheet name="Robustness" sheetId="2" r:id="rId2"/>
+    <sheet name="Retrain with subsets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Rate of noise</t>
   </si>
@@ -111,6 +112,24 @@
   </si>
   <si>
     <t>0.06, 0.04</t>
+  </si>
+  <si>
+    <t>Combination of training samples</t>
+  </si>
+  <si>
+    <t>Standard deviation of test accuracy</t>
+  </si>
+  <si>
+    <t>1: low confidence, low misliead</t>
+  </si>
+  <si>
+    <t>2: high confidence, low mislead</t>
+  </si>
+  <si>
+    <t>3: low confidence, high mislead</t>
+  </si>
+  <si>
+    <t>4: high confidence, high mislead</t>
   </si>
 </sst>
 </file>
@@ -709,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -848,4 +867,128 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="64.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.52159999999999995</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.45729999999999998</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.3639</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.18609999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0.65780000000000005</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.88080000000000003</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.70230000000000004</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.11409999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.41070000000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1.18E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.35110000000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.30859999999999999</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.1799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.64480000000000004</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.7000000000000002E-3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.75619999999999998</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.505</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.15920000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add retraining results with subsets and noise
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="67">
   <si>
     <t>Rate of noise</t>
   </si>
@@ -202,7 +202,40 @@
     <t>Mixed Gaussian random noise</t>
   </si>
   <si>
-    <t>Note: uniformly distributed random noise [0, 255]. Each subgroup has half the original training samples</t>
+    <t>Training samples</t>
+  </si>
+  <si>
+    <t>1: low confidence + low mislead</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage = 25%. </t>
+  </si>
+  <si>
+    <t>Percentage = 25%. 5x uniformly distributed random noise [0, 255]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage = 50%. </t>
+  </si>
+  <si>
+    <t>Percentage = 50%, 5x uniformly distributed random noise [0, 255]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage = 75%. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage = 75%. 5x uniformly distributed random noise [0, 255] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage = 80%. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage = 80%. 5x uniformly distributed random noise [0, 255] </t>
+  </si>
+  <si>
+    <t>Shape = [32, 32, 3, 5x]; mus = 64:32:192; sigmas = 32; scorrs = 1; filtermode = 0</t>
+  </si>
+  <si>
+    <t>Shape = [32, 32, 3, 5x]; mus = 64:32:192; sigmas = 32; scorrs = 1; filtermode = 1</t>
   </si>
 </sst>
 </file>
@@ -246,15 +279,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -266,6 +292,12 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,1407 +603,1455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="A15:XFD15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="5" customWidth="1"/>
-    <col min="9" max="9" width="30.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="9.140625" style="5"/>
-    <col min="15" max="15" width="13.5703125" style="5" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="5" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" style="5" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="27.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="13.5703125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="21.85546875" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="O1" s="4" t="s">
+      <c r="I1" s="1"/>
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="6">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="2">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="4">
         <v>0.83220000000000005</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4">
         <v>0.59389999999999998</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="4">
         <v>0.16489999999999999</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="4">
         <v>0.74890000000000001</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="4">
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="2">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>0.83509999999999995</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>0.59309999999999996</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="4">
         <v>0.1661</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="2">
         <v>0.16</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="4">
         <v>0.74890000000000001</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="4">
         <v>4.8999999999999998E-3</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <v>0.75160000000000005</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <v>3.8E-3</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>0.84140000000000004</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>0.59609999999999996</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>0.16589999999999999</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="2">
         <v>0.04</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="4">
         <v>0.75160000000000005</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="4">
         <v>3.3E-3</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>0.75180000000000002</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="2">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="4">
         <v>0.75170000000000003</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="4">
         <v>4.5999999999999999E-3</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="2">
         <v>0.75160000000000005</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="2">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>0.84189999999999998</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>0.59509999999999996</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4">
         <v>0.1663</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="2">
         <v>0.1</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="4">
         <v>0.75160000000000005</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="4">
         <v>3.8E-3</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="2">
         <v>0.752</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="2">
         <v>4.5999999999999999E-3</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>0.84209999999999996</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>0.5927</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>0.16669999999999999</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="2">
         <v>0.08</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="4">
         <v>0.75049999999999994</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="3">
         <v>12000</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="4">
         <v>0.75160000000000005</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="4">
         <v>4.1000000000000003E-3</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="2">
         <v>0.75290000000000001</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="2">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="3">
         <v>13000</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="4">
         <v>0.72250000000000003</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="2">
         <v>0.75190000000000001</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="2">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="3">
         <v>14000</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="4">
         <v>0.75249999999999995</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="2">
         <v>0.7429</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="2">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="3">
         <v>15000</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="4">
         <v>0.752</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:17" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="4">
         <v>0.74260000000000004</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>0.83230000000000004</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="4">
         <v>0.59089999999999998</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4">
         <v>0.16500000000000001</v>
       </c>
-      <c r="H16" s="5">
+      <c r="H16" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="4">
         <v>0.7419</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>5.7000000000000002E-3</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>0.8427</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>0.59060000000000001</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <v>0.16450000000000001</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="4">
         <v>0.74109999999999998</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="4">
         <v>6.3E-3</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="4">
         <v>0.83309999999999995</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="4">
         <v>0.59</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="4">
         <v>0.1646</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="4">
         <v>0.73860000000000003</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <v>0.83809999999999996</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="4">
         <v>0.58740000000000003</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="4">
         <v>0.16470000000000001</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="4">
         <v>0.73760000000000003</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>0.82820000000000005</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="4">
         <v>0.58709999999999996</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="4">
         <v>0.16450000000000001</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="5"/>
+      <c r="B21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="4">
         <v>0.73680000000000001</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>0.82030000000000003</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <v>0.58130000000000004</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4">
         <v>0.1653</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2">
         <v>50</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="4">
         <v>0.74260000000000004</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>0.83230000000000004</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="4">
         <v>0.59089999999999998</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="4">
         <v>0.16500000000000001</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="5">
+      <c r="A26" s="5"/>
+      <c r="B26" s="2">
         <v>60</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="4">
         <v>0.74339999999999995</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="4">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="4">
         <v>0.83260000000000001</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="4">
         <v>0.58240000000000003</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="4">
         <v>0.16450000000000001</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="5">
+      <c r="A27" s="5"/>
+      <c r="B27" s="2">
         <v>70</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="4">
         <v>0.74460000000000004</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="4">
         <v>0.83979999999999999</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="4">
         <v>0.59209999999999996</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="4">
         <v>0.1643</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="5">
+      <c r="A28" s="5"/>
+      <c r="B28" s="2">
         <v>80</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="4">
         <v>0.74370000000000003</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="4">
         <v>0.8478</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="4">
         <v>0.59240000000000004</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="4">
         <v>0.1643</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="5">
+      <c r="A29" s="5"/>
+      <c r="B29" s="2">
         <v>90</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="4">
         <v>0.74299999999999999</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="4">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="4">
         <v>0.84150000000000003</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="4">
         <v>0.59199999999999997</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="4">
         <v>0.1646</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="5">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2">
         <v>100</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="4">
         <v>0.74299999999999999</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="4">
         <v>6.4000000000000003E-3</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="4">
         <v>0.83919999999999995</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="4">
         <v>0.59179999999999999</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="4">
         <v>0.1646</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E33" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F33" s="4" t="s">
+      <c r="F33" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="G33" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H33" s="4" t="s">
+      <c r="H33" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="6"/>
+      <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="4">
         <v>0.74970000000000003</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="4">
         <v>0.84489999999999998</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="4">
         <v>0.59440000000000004</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="4">
         <v>0.1648</v>
       </c>
-      <c r="H34" s="5">
+      <c r="H34" s="2">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="4">
         <v>0.75149999999999995</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="4">
         <v>0.83960000000000001</v>
       </c>
-      <c r="F35" s="7">
+      <c r="F35" s="4">
         <v>0.59640000000000004</v>
       </c>
-      <c r="G35" s="7">
+      <c r="G35" s="4">
         <v>0.16539999999999999</v>
       </c>
-      <c r="H35" s="5">
+      <c r="H35" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="6"/>
+      <c r="B36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="4">
         <v>0.75129999999999997</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D36" s="4">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="4">
         <v>0.84589999999999999</v>
       </c>
-      <c r="F36" s="7">
+      <c r="F36" s="4">
         <v>0.5958</v>
       </c>
-      <c r="G36" s="7">
+      <c r="G36" s="4">
         <v>0.16619999999999999</v>
       </c>
-      <c r="H36" s="5">
+      <c r="H36" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="4">
         <v>0.75260000000000005</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="4">
         <v>4.1999999999999997E-3</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="4">
         <v>0.83989999999999998</v>
       </c>
-      <c r="F37" s="7">
+      <c r="F37" s="4">
         <v>0.59509999999999996</v>
       </c>
-      <c r="G37" s="7">
+      <c r="G37" s="4">
         <v>0.1663</v>
       </c>
-      <c r="H37" s="5">
+      <c r="H37" s="2">
         <v>0.04</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="6"/>
+      <c r="B38" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="4">
         <v>0.75209999999999999</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E38" s="4">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F38" s="4">
         <v>0.59409999999999996</v>
       </c>
-      <c r="G38" s="7">
+      <c r="G38" s="4">
         <v>0.16619999999999999</v>
       </c>
-      <c r="H38" s="5">
+      <c r="H38" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="5" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="4">
         <v>0.75160000000000005</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D39" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="4">
         <v>0.84009999999999996</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="4">
         <v>0.5917</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="4">
         <v>0.16700000000000001</v>
       </c>
-      <c r="H39" s="5">
+      <c r="H39" s="2">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="5" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="4">
         <v>0.75280000000000002</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D40" s="4">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="4">
         <v>0.83250000000000002</v>
       </c>
-      <c r="F40" s="7">
+      <c r="F40" s="4">
         <v>0.58499999999999996</v>
       </c>
-      <c r="G40" s="7">
+      <c r="G40" s="4">
         <v>0.16930000000000001</v>
       </c>
-      <c r="H40" s="5">
+      <c r="H40" s="2">
         <v>0.32</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="5" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="4">
         <v>0.75290000000000001</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D41" s="4">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="4">
         <v>0.81799999999999995</v>
       </c>
-      <c r="F41" s="7">
+      <c r="F41" s="4">
         <v>0.56989999999999996</v>
       </c>
-      <c r="G41" s="7">
+      <c r="G41" s="4">
         <v>0.17269999999999999</v>
       </c>
-      <c r="H41" s="5">
+      <c r="H41" s="2">
         <v>0.22</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="5" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="4">
         <v>0.74709999999999999</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D42" s="4">
         <v>3.8E-3</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="4">
         <v>0.80369999999999997</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F42" s="4">
         <v>0.5454</v>
       </c>
-      <c r="G42" s="7">
+      <c r="G42" s="4">
         <v>0.1772</v>
       </c>
-      <c r="H42" s="5">
+      <c r="H42" s="2">
         <v>0.22</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="D46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E46" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F46" s="4" t="s">
+      <c r="F46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="4" t="s">
+      <c r="G46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="4" t="s">
+      <c r="H46" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="5">
+      <c r="A47" s="6"/>
+      <c r="B47" s="2">
         <v>50</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="4">
         <v>0.74839999999999995</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D47" s="4">
         <v>4.8999999999999998E-3</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="4">
         <v>0.82820000000000005</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F47" s="4">
         <v>0.59299999999999997</v>
       </c>
-      <c r="G47" s="7">
+      <c r="G47" s="4">
         <v>0.1656</v>
       </c>
-      <c r="H47" s="5">
+      <c r="H47" s="2">
         <v>0.32</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="5">
+      <c r="A48" s="6"/>
+      <c r="B48" s="2">
         <v>60</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C48" s="4">
         <v>0.74819999999999998</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D48" s="4">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="4">
         <v>0.84599999999999997</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F48" s="4">
         <v>0.59389999999999998</v>
       </c>
-      <c r="G48" s="7">
+      <c r="G48" s="4">
         <v>0.16589999999999999</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H48" s="2">
         <v>0.3</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="5">
+      <c r="A49" s="6"/>
+      <c r="B49" s="2">
         <v>70</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C49" s="4">
         <v>0.74970000000000003</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D49" s="4">
         <v>5.1000000000000004E-3</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="4">
         <v>0.84489999999999998</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F49" s="4">
         <v>0.59440000000000004</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="4">
         <v>0.1648</v>
       </c>
-      <c r="H49" s="5">
+      <c r="H49" s="2">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="5">
+      <c r="A50" s="6"/>
+      <c r="B50" s="2">
         <v>80</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="4">
         <v>0.74819999999999998</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D50" s="4">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="4">
         <v>0.83740000000000003</v>
       </c>
-      <c r="F50" s="7">
+      <c r="F50" s="4">
         <v>0.59299999999999997</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G50" s="4">
         <v>0.1658</v>
       </c>
-      <c r="H50" s="5">
+      <c r="H50" s="2">
         <v>0.12</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="5">
+      <c r="A51" s="6"/>
+      <c r="B51" s="2">
         <v>90</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="4">
         <v>0.74929999999999997</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D51" s="4">
         <v>5.3E-3</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="4">
         <v>0.84179999999999999</v>
       </c>
-      <c r="F51" s="7">
+      <c r="F51" s="4">
         <v>0.59379999999999999</v>
       </c>
-      <c r="G51" s="7">
+      <c r="G51" s="4">
         <v>0.1651</v>
       </c>
-      <c r="H51" s="5">
+      <c r="H51" s="2">
         <v>0.16</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="5">
+      <c r="A52" s="6"/>
+      <c r="B52" s="2">
         <v>100</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="4">
         <v>0.74809999999999999</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="4">
         <v>4.4000000000000003E-3</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="4">
         <v>0.84019999999999995</v>
       </c>
-      <c r="F52" s="7">
+      <c r="F52" s="4">
         <v>0.59470000000000001</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G52" s="4">
         <v>0.16489999999999999</v>
       </c>
-      <c r="H52" s="5">
+      <c r="H52" s="2">
         <v>0.12</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="5">
+      <c r="A53" s="6"/>
+      <c r="B53" s="2">
         <v>150</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="4">
         <v>0.74950000000000006</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="4">
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="4">
         <v>0.84360000000000002</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F53" s="4">
         <v>0.59560000000000002</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G53" s="4">
         <v>0.1651</v>
       </c>
-      <c r="H53" s="5">
+      <c r="H53" s="2">
         <v>0.26</v>
       </c>
     </row>
-    <row r="56" spans="1:8" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:8" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C56" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D56" s="4" t="s">
+      <c r="D56" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E56" s="4" t="s">
+      <c r="E56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F56" s="4" t="s">
+      <c r="F56" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G56" s="4" t="s">
+      <c r="G56" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H56" s="4" t="s">
+      <c r="H56" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="5" t="s">
+      <c r="A57" s="5"/>
+      <c r="B57" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="4">
         <v>0.75209999999999999</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D57" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="4">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="4">
         <v>0.59409999999999996</v>
       </c>
-      <c r="G57" s="7">
+      <c r="G57" s="4">
         <v>0.16619999999999999</v>
       </c>
-      <c r="H57" s="5">
+      <c r="H57" s="2">
         <v>0.06</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-      <c r="B58" s="5">
+      <c r="A58" s="5"/>
+      <c r="B58" s="2">
         <v>3</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="4">
         <v>0.75029999999999997</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D58" s="4">
         <v>4.7000000000000002E-3</v>
       </c>
-      <c r="E58" s="7">
+      <c r="E58" s="4">
         <v>0.84140000000000004</v>
       </c>
-      <c r="F58" s="7">
+      <c r="F58" s="4">
         <v>0.59289999999999998</v>
       </c>
-      <c r="G58" s="7">
+      <c r="G58" s="4">
         <v>0.16669999999999999</v>
       </c>
-      <c r="H58" s="5">
+      <c r="H58" s="2">
         <v>0.54</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="5">
+      <c r="A59" s="5"/>
+      <c r="B59" s="2">
         <v>5</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C59" s="4">
         <v>0.74439999999999995</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D59" s="4">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="4">
         <v>0.83609999999999995</v>
       </c>
-      <c r="F59" s="7">
+      <c r="F59" s="4">
         <v>0.58979999999999999</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="4">
         <v>0.1668</v>
       </c>
-      <c r="H59" s="5">
+      <c r="H59" s="2">
         <v>1.52</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="5">
+      <c r="A60" s="5"/>
+      <c r="B60" s="2">
         <v>7</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="4">
         <v>0.74299999999999999</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D60" s="4">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="4">
         <v>0.82940000000000003</v>
       </c>
-      <c r="F60" s="7">
+      <c r="F60" s="4">
         <v>0.58819999999999995</v>
       </c>
-      <c r="G60" s="7">
+      <c r="G60" s="4">
         <v>0.16639999999999999</v>
       </c>
-      <c r="H60" s="5">
+      <c r="H60" s="2">
         <v>1.6</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="5" t="s">
+      <c r="A61" s="5"/>
+      <c r="B61" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="5">
+      <c r="A62" s="5"/>
+      <c r="B62" s="2">
         <v>3</v>
       </c>
-      <c r="C62" s="7">
+      <c r="C62" s="4">
         <v>0.75070000000000003</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D62" s="4">
         <v>4.1000000000000003E-3</v>
       </c>
-      <c r="E62" s="7">
+      <c r="E62" s="4">
         <v>0.83850000000000002</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F62" s="4">
         <v>0.59370000000000001</v>
       </c>
-      <c r="G62" s="7">
+      <c r="G62" s="4">
         <v>0.16689999999999999</v>
       </c>
-      <c r="H62" s="5">
+      <c r="H62" s="2">
         <v>0.52</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="5">
+      <c r="A63" s="5"/>
+      <c r="B63" s="2">
         <v>5</v>
       </c>
-      <c r="C63" s="7">
+      <c r="C63" s="4">
         <v>0.74790000000000001</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D63" s="4">
         <v>5.4000000000000003E-3</v>
       </c>
-      <c r="E63" s="7">
+      <c r="E63" s="4">
         <v>0.83789999999999998</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F63" s="4">
         <v>0.59330000000000005</v>
       </c>
-      <c r="G63" s="7">
+      <c r="G63" s="4">
         <v>0.16689999999999999</v>
       </c>
-      <c r="H63" s="5">
+      <c r="H63" s="2">
         <v>2.1</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="3"/>
-      <c r="B64" s="5">
+      <c r="A64" s="5"/>
+      <c r="B64" s="2">
         <v>7</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="4">
         <v>0.74560000000000004</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D64" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="E64" s="7">
+      <c r="E64" s="4">
         <v>0.84040000000000004</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F64" s="4">
         <v>0.59150000000000003</v>
       </c>
-      <c r="G64" s="7">
+      <c r="G64" s="4">
         <v>0.1668</v>
       </c>
-      <c r="H64" s="5">
+      <c r="H64" s="2">
         <v>2.54</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="C67" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="D67" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E67" s="4" t="s">
+      <c r="E67" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F67" s="4" t="s">
+      <c r="F67" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G67" s="4" t="s">
+      <c r="G67" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H67" s="4" t="s">
+      <c r="H67" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A68" s="3"/>
-      <c r="B68" s="5" t="s">
+      <c r="A68" s="5"/>
+      <c r="B68" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="4">
         <v>0.73880000000000001</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D68" s="4">
         <v>5.1999999999999998E-3</v>
       </c>
-      <c r="E68" s="7">
+      <c r="E68" s="4">
         <v>0.82399999999999995</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F68" s="4">
         <v>0.58860000000000001</v>
       </c>
-      <c r="G68" s="7">
+      <c r="G68" s="4">
         <v>0.16439999999999999</v>
       </c>
-      <c r="H68" s="5">
+      <c r="H68" s="2">
         <v>5.56</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="A69" s="3"/>
-      <c r="B69" s="5" t="s">
+      <c r="A69" s="5"/>
+      <c r="B69" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C69" s="7">
+      <c r="C69" s="4">
         <v>0.73680000000000001</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D69" s="4">
         <v>5.5999999999999999E-3</v>
       </c>
-      <c r="E69" s="7">
+      <c r="E69" s="4">
         <v>0.8367</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F69" s="4">
         <v>0.58730000000000004</v>
       </c>
-      <c r="G69" s="7">
+      <c r="G69" s="4">
         <v>0.16500000000000001</v>
       </c>
-      <c r="H69" s="5">
+      <c r="H69" s="2">
         <v>3.18</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C70" s="4">
+        <v>0.74709999999999999</v>
+      </c>
+      <c r="D70" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E70" s="4">
+        <v>0.8337</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0.59450000000000003</v>
+      </c>
+      <c r="G70" s="4">
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C71" s="4">
+        <v>0.748</v>
+      </c>
+      <c r="D71" s="4">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="E71" s="4">
+        <v>0.84570000000000001</v>
+      </c>
+      <c r="F71" s="4">
+        <v>0.59440000000000004</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0.1646</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0.14000000000000001</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A67:A69"/>
     <mergeCell ref="A1:A11"/>
     <mergeCell ref="A15:A21"/>
     <mergeCell ref="A24:A30"/>
     <mergeCell ref="A33:A42"/>
     <mergeCell ref="A46:A53"/>
     <mergeCell ref="A56:A64"/>
+    <mergeCell ref="A67:A71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1980,128 +2060,950 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:P34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="2"/>
+    <col min="2" max="2" width="32.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" style="2"/>
+    <col min="4" max="4" width="20.140625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="17.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="I1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="4">
         <v>0.52159999999999995</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="4">
         <v>1.5800000000000002E-2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="4">
         <v>0.45729999999999998</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="4">
         <v>0.3639</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="4">
         <v>0.18609999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.53110000000000002</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0.37259999999999999</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0.1923</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="4">
         <v>0.65780000000000005</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="4">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="4">
         <v>0.88080000000000003</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="4">
         <v>0.70230000000000004</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="4">
         <v>0.11409999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0.66369999999999996</v>
+      </c>
+      <c r="L3" s="4">
+        <v>5.3E-3</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0.88560000000000005</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0.70030000000000003</v>
+      </c>
+      <c r="O3" s="4">
+        <v>0.11609999999999999</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="4">
         <v>0.41070000000000001</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="4">
         <v>1.18E-2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="4">
         <v>0.35110000000000002</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="4">
         <v>0.30859999999999999</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="4">
         <v>0.1799</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0.40820000000000001</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.01E-2</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0.35049999999999998</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0.31230000000000002</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0.1855</v>
+      </c>
+      <c r="P4" s="2">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="4">
         <v>0.64480000000000004</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="4">
         <v>6.7000000000000002E-3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="4">
         <v>0.75619999999999998</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="4">
         <v>0.505</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="4">
         <v>0.15920000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="4">
+        <v>0.65129999999999999</v>
+      </c>
+      <c r="L5" s="4">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0.50470000000000004</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0.16159999999999999</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:16" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="K10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.2712</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.2656</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.2291</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.14649999999999999</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.30819999999999997</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2.1100000000000001E-2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.28310000000000002</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0.2414</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.15429999999999999</v>
+      </c>
+      <c r="P11" s="2">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.53610000000000002</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.23E-2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.79669999999999996</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G12" s="4">
+        <v>0.1273</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0.55269999999999997</v>
+      </c>
+      <c r="L12" s="4">
+        <v>8.6E-3</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0.79239999999999999</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0.58599999999999997</v>
+      </c>
+      <c r="O12" s="4">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="P12" s="2">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.19259999999999999</v>
+      </c>
+      <c r="D13" s="4">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.24679999999999999</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.2286</v>
+      </c>
+      <c r="G13" s="4">
+        <v>0.13669999999999999</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0.2132</v>
+      </c>
+      <c r="L13" s="4">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0.25269999999999998</v>
+      </c>
+      <c r="N13" s="4">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="O13" s="4">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="P13" s="2">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.51490000000000002</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.29E-2</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.66569999999999996</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.44769999999999999</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0.1457</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="4">
+        <v>0.53180000000000005</v>
+      </c>
+      <c r="L14" s="4">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0.67379999999999995</v>
+      </c>
+      <c r="N14" s="4">
+        <v>0.4481</v>
+      </c>
+      <c r="O14" s="4">
+        <v>0.14829999999999999</v>
+      </c>
+      <c r="P14" s="2">
+        <v>3.68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15" s="6"/>
+      <c r="K15" s="4">
+        <v>0.53259999999999996</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1.06E-2</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0.67220000000000002</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0.4481</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0.1487</v>
+      </c>
+      <c r="P15" s="2">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.68759999999999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="E22" s="4">
+        <v>0.74250000000000005</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.52339999999999998</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0.18360000000000001</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K22" s="4">
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="L22" s="4">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0.73880000000000001</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0.53259999999999996</v>
+      </c>
+      <c r="O22" s="4">
+        <v>0.1842</v>
+      </c>
+      <c r="P22" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.70809999999999995</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3.0999999999999999E-3</v>
+      </c>
+      <c r="E23" s="4">
+        <v>0.92669999999999997</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.76090000000000002</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0.1028</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0.71050000000000002</v>
+      </c>
+      <c r="L23" s="4">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0.92430000000000001</v>
+      </c>
+      <c r="N23" s="4">
+        <v>0.75639999999999996</v>
+      </c>
+      <c r="O23" s="4">
+        <v>0.10539999999999999</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.60550000000000004</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0.58330000000000004</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.43</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0.20330000000000001</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0.61950000000000005</v>
+      </c>
+      <c r="L24" s="4">
+        <v>1.38E-2</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0.54949999999999999</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0.438</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0.2069</v>
+      </c>
+      <c r="P24" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.70850000000000002</v>
+      </c>
+      <c r="D25" s="4">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="E25" s="4">
+        <v>0.80449999999999999</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.55759999999999998</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0.16239999999999999</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" s="4">
+        <v>0.71419999999999995</v>
+      </c>
+      <c r="L25" s="4">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0.80940000000000001</v>
+      </c>
+      <c r="N25" s="4">
+        <v>0.5575</v>
+      </c>
+      <c r="O25" s="4">
+        <v>0.1648</v>
+      </c>
+      <c r="P25" s="2">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="1" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.70889999999999997</v>
+      </c>
+      <c r="D30" s="4">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="E30" s="4">
+        <v>0.77039999999999997</v>
+      </c>
+      <c r="F30" s="4">
+        <v>0.5494</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0.1779</v>
+      </c>
+      <c r="I30" s="5"/>
+      <c r="J30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="K30" s="4">
+        <v>0.71679999999999999</v>
+      </c>
+      <c r="L30" s="4">
+        <v>7.9000000000000008E-3</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0.79039999999999999</v>
+      </c>
+      <c r="N30" s="4">
+        <v>0.55320000000000003</v>
+      </c>
+      <c r="O30" s="4">
+        <v>0.1789</v>
+      </c>
+      <c r="P30" s="2">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.71430000000000005</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="E31" s="4">
+        <v>0.92649999999999999</v>
+      </c>
+      <c r="F31" s="4">
+        <v>0.76729999999999998</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0.1016</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.71760000000000002</v>
+      </c>
+      <c r="L31" s="4">
+        <v>2.8E-3</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0.92290000000000005</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0.76359999999999995</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0.10440000000000001</v>
+      </c>
+      <c r="P31" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.64119999999999999</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0.6099</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0.46060000000000001</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0.2009</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K32" s="4">
+        <v>0.65210000000000001</v>
+      </c>
+      <c r="L32" s="4">
+        <v>1.61E-2</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0.6381</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0.46510000000000001</v>
+      </c>
+      <c r="O32" s="4">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="P32" s="2">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="4">
+        <v>0.6421</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="F33" s="4">
+        <v>0.4627</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K33" s="4">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="L33" s="4">
+        <v>4.3E-3</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0.81730000000000003</v>
+      </c>
+      <c r="N33" s="4">
+        <v>0.56740000000000002</v>
+      </c>
+      <c r="O33" s="4">
+        <v>0.1651</v>
+      </c>
+      <c r="P33" s="2">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.71750000000000003</v>
+      </c>
+      <c r="D34" s="4">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0.82450000000000001</v>
+      </c>
+      <c r="F34" s="4">
+        <v>0.56569999999999998</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0.16320000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="I21:I25"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="I29:I33"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A1:A5"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="I10:I14"/>
+    <mergeCell ref="I1:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>